<commit_message>
Modify requirements and comparer
</commit_message>
<xml_diff>
--- a/output_files/OFAC_Transfer_2025-03-05.xlsx
+++ b/output_files/OFAC_Transfer_2025-03-05.xlsx
@@ -437,7 +437,7 @@
     <col width="58" customWidth="1" min="2" max="2"/>
     <col width="14" customWidth="1" min="3" max="3"/>
     <col width="19" customWidth="1" min="4" max="4"/>
-    <col width="52" customWidth="1" min="5" max="5"/>
+    <col width="57" customWidth="1" min="5" max="5"/>
     <col width="19" customWidth="1" min="6" max="6"/>
   </cols>
   <sheetData>
@@ -530,7 +530,7 @@
         </is>
       </c>
       <c r="F3" t="n">
-        <v>46.9982533708221</v>
+        <v>28.57142857142857</v>
       </c>
     </row>
     <row r="4">
@@ -551,16 +551,16 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>26529</t>
+          <t>52112</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>ANSAR INFORMATION TECHNOLOGY COMPANY</t>
+          <t>SICHUAN SILENCE INFORMATION TECHNOLOGY COMPANY, LIMITED</t>
         </is>
       </c>
       <c r="F4" t="n">
-        <v>46.6769419998417</v>
+        <v>55.07246376811595</v>
       </c>
     </row>
     <row r="5">
@@ -581,16 +581,16 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>6939</t>
+          <t>21558</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>AL-AHDAL, Mohammad Hamdi Mohammad Sadiq</t>
+          <t>MAGHAM, Mohammad</t>
         </is>
       </c>
       <c r="F5" t="n">
-        <v>29.33166060522351</v>
+        <v>45.45454545454545</v>
       </c>
     </row>
     <row r="6">
@@ -611,16 +611,16 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>17291</t>
+          <t>17292</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>ABD AL-SALAM, 'Abd al-Malik Muhammad Yusuf 'Uthman</t>
+          <t>ABD AL-SALAM, Ashraf Muhammad Yusuf 'Uthman</t>
         </is>
       </c>
       <c r="F6" t="n">
-        <v>73.14482026746586</v>
+        <v>45.23809523809524</v>
       </c>
     </row>
     <row r="7">
@@ -641,16 +641,16 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>17387</t>
+          <t>6915</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>SALEH, Ali Abdullah</t>
+          <t>ABDULLAH, Abdullah Ahmed</t>
         </is>
       </c>
       <c r="F7" t="n">
-        <v>50.08739836330069</v>
+        <v>36.58536585365854</v>
       </c>
     </row>
     <row r="8">
@@ -671,16 +671,16 @@
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>46816</t>
+          <t>6915</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>SALAH, Salah Abdallah Mohamed</t>
+          <t>ABDULLAH, Abdullah Ahmed</t>
         </is>
       </c>
       <c r="F8" t="n">
-        <v>40.07379809165462</v>
+        <v>37.83783783783784</v>
       </c>
     </row>
     <row r="9">
@@ -701,16 +701,16 @@
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>26862</t>
+          <t>39261</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>SALIH AL HASANI, Mohammed Hussein</t>
+          <t>SALAD, Mohamed Hussein</t>
         </is>
       </c>
       <c r="F9" t="n">
-        <v>41.51173714314132</v>
+        <v>37.83783783783784</v>
       </c>
     </row>
     <row r="10">
@@ -740,7 +740,7 @@
         </is>
       </c>
       <c r="F10" t="n">
-        <v>38.4239342119448</v>
+        <v>27.77777777777778</v>
       </c>
     </row>
     <row r="11">
@@ -770,7 +770,7 @@
         </is>
       </c>
       <c r="F11" t="n">
-        <v>38.4239342119448</v>
+        <v>27.77777777777778</v>
       </c>
     </row>
     <row r="12">
@@ -791,16 +791,16 @@
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>6365</t>
+          <t>39261</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>BIN LADIN, Usama bin Muhammad bin Awad</t>
+          <t>SALAD, Mohamed Hussein</t>
         </is>
       </c>
       <c r="F12" t="n">
-        <v>55.42018879086922</v>
+        <v>30.23255813953488</v>
       </c>
     </row>
     <row r="13">
@@ -821,16 +821,16 @@
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>26862</t>
+          <t>39261</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>SALIH AL HASANI, Mohammed Hussein</t>
+          <t>SALAD, Mohamed Hussein</t>
         </is>
       </c>
       <c r="F13" t="n">
-        <v>41.51173714314132</v>
+        <v>37.83783783783784</v>
       </c>
     </row>
     <row r="14">
@@ -851,16 +851,16 @@
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>29843</t>
+          <t>9660</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>MEHRI, Mahdi</t>
+          <t>FARHAT, Mariam Mohammed</t>
         </is>
       </c>
       <c r="F14" t="n">
-        <v>36.21110445268626</v>
+        <v>41.37931034482759</v>
       </c>
     </row>
     <row r="15">
@@ -881,16 +881,16 @@
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>7877</t>
+          <t>29843</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>AL-SALIH, Muhammad Mahdi</t>
+          <t>MEHRI, Mahdi</t>
         </is>
       </c>
       <c r="F15" t="n">
-        <v>46.86012163117363</v>
+        <v>26.31578947368421</v>
       </c>
     </row>
     <row r="16">
@@ -911,16 +911,16 @@
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>17927</t>
+          <t>39316</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>AL HOUTHI, Abdul Malik</t>
+          <t>BADAAS, Mohamed Ali</t>
         </is>
       </c>
       <c r="F16" t="n">
-        <v>53.52986900003602</v>
+        <v>42.30769230769231</v>
       </c>
     </row>
     <row r="17">
@@ -941,16 +941,16 @@
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>17927</t>
+          <t>24035</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>AL HOUTHI, Abdul Malik</t>
+          <t>SABAHI, Mohammed Reza</t>
         </is>
       </c>
       <c r="F17" t="n">
-        <v>53.52986900003602</v>
+        <v>37.93103448275862</v>
       </c>
     </row>
     <row r="18">
@@ -971,16 +971,16 @@
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>21992</t>
+          <t>52308</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>AL-'ALI, Salih</t>
+          <t>AL-HADI, Ahmad Muhammad Muhammad Hasan</t>
         </is>
       </c>
       <c r="F18" t="n">
-        <v>63.19550135446739</v>
+        <v>44.73684210526316</v>
       </c>
     </row>
     <row r="19">
@@ -1001,16 +1001,16 @@
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>13126</t>
+          <t>50667</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>HADI, Abdul</t>
+          <t>ABDI, Ali</t>
         </is>
       </c>
       <c r="F19" t="n">
-        <v>60.05218765754926</v>
+        <v>41.66666666666667</v>
       </c>
     </row>
     <row r="20">
@@ -1031,16 +1031,16 @@
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>6927</t>
+          <t>43061</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>MOHAMMED, Fazul Abdullah</t>
+          <t>HIREY, Mohamed Abdullah</t>
         </is>
       </c>
       <c r="F20" t="n">
-        <v>38.69100777246381</v>
+        <v>32.5</v>
       </c>
     </row>
     <row r="21">
@@ -1070,7 +1070,7 @@
         </is>
       </c>
       <c r="F21" t="n">
-        <v>58.56590402927218</v>
+        <v>46.15384615384615</v>
       </c>
     </row>
     <row r="22">
@@ -1091,16 +1091,16 @@
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>17291</t>
+          <t>46188</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>ABD AL-SALAM, 'Abd al-Malik Muhammad Yusuf 'Uthman</t>
+          <t>AL-AJOURI, Akram</t>
         </is>
       </c>
       <c r="F22" t="n">
-        <v>56.72680159251951</v>
+        <v>22.22222222222222</v>
       </c>
     </row>
     <row r="23">
@@ -1121,16 +1121,16 @@
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>50721</t>
+          <t>30167</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>BARAKAT, Khaled</t>
+          <t>GUL, Redi Hussein Khal</t>
         </is>
       </c>
       <c r="F23" t="n">
-        <v>32.36239903300242</v>
+        <v>29.41176470588236</v>
       </c>
     </row>
     <row r="24">
@@ -1151,16 +1151,16 @@
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>21952</t>
+          <t>18600</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>HUSAYN, 'Ali</t>
+          <t>AL-SHA'IRI, Husayn Al-Salihin Salih</t>
         </is>
       </c>
       <c r="F24" t="n">
-        <v>37.58562815735084</v>
+        <v>26.19047619047619</v>
       </c>
     </row>
     <row r="25">
@@ -1181,16 +1181,16 @@
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>21952</t>
+          <t>45128</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>HUSAYN, 'Ali</t>
+          <t>HANAFI, Khalid</t>
         </is>
       </c>
       <c r="F25" t="n">
-        <v>41.64445249979061</v>
+        <v>30.43478260869566</v>
       </c>
     </row>
     <row r="26">
@@ -1211,16 +1211,16 @@
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>6915</t>
+          <t>39296</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>ABDULLAH, Abdullah Ahmed</t>
+          <t>JEERI, Abdullahi</t>
         </is>
       </c>
       <c r="F26" t="n">
-        <v>34.4749704040991</v>
+        <v>22.22222222222222</v>
       </c>
     </row>
     <row r="27">
@@ -1241,16 +1241,16 @@
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>16557</t>
+          <t>17789</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>ISHAQ, Malik</t>
+          <t>TAHINI, Abdallah Asad</t>
         </is>
       </c>
       <c r="F27" t="n">
-        <v>62.26276592156547</v>
+        <v>20</v>
       </c>
     </row>
     <row r="28">
@@ -1271,16 +1271,16 @@
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>20947</t>
+          <t>20882</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>AL-HASAN, Suhayl Hasan</t>
+          <t>JASHARI, Abdul</t>
         </is>
       </c>
       <c r="F28" t="n">
-        <v>33.61400225709856</v>
+        <v>21.875</v>
       </c>
     </row>
     <row r="29">
@@ -1301,16 +1301,16 @@
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>23054</t>
+          <t>49358</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>AL-YAFI'I, Nashwan al-Wali</t>
+          <t>AL-WAZIR, Ali Abd-Al-Wahhab Muhammad</t>
         </is>
       </c>
       <c r="F29" t="n">
-        <v>48.14514028444156</v>
+        <v>23.25581395348837</v>
       </c>
     </row>
     <row r="30">
@@ -1331,16 +1331,16 @@
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>13125</t>
+          <t>13157</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>WALI, Mohammad</t>
+          <t>BARI, Abdul Baqi</t>
         </is>
       </c>
       <c r="F30" t="n">
-        <v>49.9084955421776</v>
+        <v>33.33333333333333</v>
       </c>
     </row>
     <row r="31">
@@ -1361,16 +1361,16 @@
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>50097</t>
+          <t>29269</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>K F D GENERAL TRADING L.L.C</t>
+          <t>ADAM TRADING AND INVESTMENT LLC</t>
         </is>
       </c>
       <c r="F31" t="n">
-        <v>50.30055157145482</v>
+        <v>46.80851063829788</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add Transfer comparison for UE
</commit_message>
<xml_diff>
--- a/output_files/OFAC_Transfer_2025-03-05.xlsx
+++ b/output_files/OFAC_Transfer_2025-03-05.xlsx
@@ -449,12 +449,12 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>Nombre</t>
+          <t>NOMBRE</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>Documento</t>
+          <t>DOCUMENTO</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">

</xml_diff>